<commit_message>
Order.java private Attribute, Fehler: User überschreibtinital User
</commit_message>
<xml_diff>
--- a/databases/DefaultUSERS.xlsx
+++ b/databases/DefaultUSERS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\Documents\GitHub Repositories\HWG Repos\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7D7678-311B-4C8F-B5CC-814BF3495874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CC15D2-4034-4FDB-82C2-67AB3DE3E69F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
   </bookViews>
@@ -33,213 +33,216 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>Max</t>
   </si>
   <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Steffanie</t>
+  </si>
+  <si>
+    <t>Luisa</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Wolfgang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hermine </t>
+  </si>
+  <si>
+    <t>Koch</t>
+  </si>
+  <si>
+    <t>Schmidt</t>
+  </si>
+  <si>
+    <t>Müller</t>
+  </si>
+  <si>
+    <t>Fuchs</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>Fischer</t>
+  </si>
+  <si>
+    <t>Bauer</t>
+  </si>
+  <si>
+    <t>Klein</t>
+  </si>
+  <si>
+    <t>Hauptstraße 3</t>
+  </si>
+  <si>
+    <t>Hauptstraße 34</t>
+  </si>
+  <si>
+    <t>Schillerstraße 6</t>
+  </si>
+  <si>
+    <t>Turmstraße 8</t>
+  </si>
+  <si>
+    <t>Königsstraße 22</t>
+  </si>
+  <si>
+    <t>Marktstraße 45</t>
+  </si>
+  <si>
+    <t>Kirchstraße 29</t>
+  </si>
+  <si>
+    <t>Rathausplatz 19</t>
+  </si>
+  <si>
+    <t>Königsbach-Stein</t>
+  </si>
+  <si>
+    <t>Pforzheim</t>
+  </si>
+  <si>
+    <t>Bietigheim-Bissingen</t>
+  </si>
+  <si>
+    <t>Sindelfingen</t>
+  </si>
+  <si>
+    <t>Böblingen</t>
+  </si>
+  <si>
+    <t>Ketsch</t>
+  </si>
+  <si>
+    <t>Ilvesheim</t>
+  </si>
+  <si>
+    <t>Remchingen</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>personnel_id</t>
+  </si>
+  <si>
+    <t>forename</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>street_nr</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>passwort123</t>
+  </si>
+  <si>
+    <t>laura.koch@example.com</t>
+  </si>
+  <si>
+    <t>luisa.fuchs@example.com</t>
+  </si>
+  <si>
+    <t>robert.fischer@example.com</t>
+  </si>
+  <si>
+    <t>wolfgang.bauer@example.com</t>
+  </si>
+  <si>
+    <t>hermine.klein@example.com</t>
+  </si>
+  <si>
+    <t>steffanie.mueller@example.com</t>
+  </si>
+  <si>
+    <t>samuel.fischer@example.com</t>
+  </si>
+  <si>
+    <t>isLoggedIn</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>laura_koch</t>
+  </si>
+  <si>
+    <t>steffanie_müller</t>
+  </si>
+  <si>
+    <t>luisa_fuchs</t>
+  </si>
+  <si>
+    <t>samuel_schneider</t>
+  </si>
+  <si>
+    <t>robert_fischer</t>
+  </si>
+  <si>
+    <t>wolfgang_bauer</t>
+  </si>
+  <si>
+    <t>hermine_klein</t>
+  </si>
+  <si>
+    <t>max_schmidt</t>
+  </si>
+  <si>
+    <t>max.schmidt@example.com</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>max_mustermann</t>
+  </si>
+  <si>
     <t>Mustermann</t>
   </si>
   <si>
+    <t>Musterstraße 1</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
     <t>Musterstadt</t>
   </si>
   <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>Steffanie</t>
-  </si>
-  <si>
-    <t>Luisa</t>
-  </si>
-  <si>
-    <t>Samuel</t>
-  </si>
-  <si>
-    <t>Robert</t>
-  </si>
-  <si>
-    <t>Wolfgang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hermine </t>
-  </si>
-  <si>
-    <t>Koch</t>
-  </si>
-  <si>
-    <t>Schmidt</t>
-  </si>
-  <si>
-    <t>Müller</t>
-  </si>
-  <si>
-    <t>Fuchs</t>
-  </si>
-  <si>
-    <t>Schneider</t>
-  </si>
-  <si>
-    <t>Fischer</t>
-  </si>
-  <si>
-    <t>Bauer</t>
-  </si>
-  <si>
-    <t>Klein</t>
-  </si>
-  <si>
-    <t>Hauptstraße 3</t>
-  </si>
-  <si>
-    <t>Hauptstraße 34</t>
-  </si>
-  <si>
-    <t>Schillerstraße 6</t>
-  </si>
-  <si>
-    <t>Turmstraße 8</t>
-  </si>
-  <si>
-    <t>Königsstraße 22</t>
-  </si>
-  <si>
-    <t>Marktstraße 45</t>
-  </si>
-  <si>
-    <t>Kirchstraße 29</t>
-  </si>
-  <si>
-    <t>Rathausplatz 19</t>
-  </si>
-  <si>
-    <t>Königsbach-Stein</t>
-  </si>
-  <si>
-    <t>Pforzheim</t>
-  </si>
-  <si>
-    <t>Bietigheim-Bissingen</t>
-  </si>
-  <si>
-    <t>Sindelfingen</t>
-  </si>
-  <si>
-    <t>Böblingen</t>
-  </si>
-  <si>
-    <t>Ketsch</t>
-  </si>
-  <si>
-    <t>Ilvesheim</t>
-  </si>
-  <si>
-    <t>Remchingen</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>personnel_id</t>
-  </si>
-  <si>
-    <t>forename</t>
-  </si>
-  <si>
-    <t>surname</t>
-  </si>
-  <si>
-    <t>street_nr</t>
-  </si>
-  <si>
-    <t>zip</t>
-  </si>
-  <si>
-    <t>role_id</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>passwort123</t>
-  </si>
-  <si>
-    <t>laura.koch@example.com</t>
-  </si>
-  <si>
-    <t>luisa.fuchs@example.com</t>
-  </si>
-  <si>
-    <t>robert.fischer@example.com</t>
-  </si>
-  <si>
-    <t>wolfgang.bauer@example.com</t>
-  </si>
-  <si>
-    <t>hermine.klein@example.com</t>
-  </si>
-  <si>
-    <t>steffanie.mueller@example.com</t>
-  </si>
-  <si>
-    <t>samuel.fischer@example.com</t>
-  </si>
-  <si>
-    <t>isLoggedIn</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>max_mustermann</t>
-  </si>
-  <si>
-    <t>laura_koch</t>
-  </si>
-  <si>
-    <t>steffanie_müller</t>
-  </si>
-  <si>
-    <t>luisa_fuchs</t>
-  </si>
-  <si>
-    <t>samuel_schneider</t>
-  </si>
-  <si>
-    <t>robert_fischer</t>
-  </si>
-  <si>
-    <t>wolfgang_bauer</t>
-  </si>
-  <si>
-    <t>hermine_klein</t>
-  </si>
-  <si>
-    <t>max_schmidt</t>
-  </si>
-  <si>
-    <t>max.schmidt@example.com</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>..._...@....</t>
-  </si>
-  <si>
-    <t>**********</t>
-  </si>
-  <si>
-    <t>Musterstraße 1</t>
-  </si>
-  <si>
-    <t>max_mustermann@example.com</t>
+    <t>max.mustermann@example.com</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -625,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E69E-E720-4C2D-B81A-DEA44878441D}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,107 +652,107 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="1">
+        <v>11111</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="3">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="3">
-        <v>12345</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -757,28 +760,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3">
         <v>75196</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
@@ -792,28 +795,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3">
         <v>68549</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
@@ -827,28 +830,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3">
         <v>68775</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J6" s="3">
         <v>2</v>
@@ -862,28 +865,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3">
         <v>71032</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J7" s="3">
         <v>1</v>
@@ -897,28 +900,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3">
         <v>71065</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J8" s="3">
         <v>1</v>
@@ -932,28 +935,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" s="3">
         <v>74321</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" s="3">
         <v>2</v>
@@ -967,28 +970,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="3">
         <v>75172</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J10" s="3">
         <v>2</v>
@@ -1002,47 +1005,33 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3">
         <v>75203</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J11" s="3">
         <v>1</v>
       </c>
       <c r="K11" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1050,19 +1039,18 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{6CCE9D38-E241-495E-B467-931EEDC3C12E}"/>
-    <hyperlink ref="H4:H11" r:id="rId2" display="max.mustermann@example.com" xr:uid="{077A01C1-E489-4149-B981-81DAB0D867CD}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{C11D9D94-AD0C-46DA-A6DD-3C7F0E2C9559}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{6EE26CD2-963C-4EF1-8815-7C2C179EE829}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{FCB8C551-BF70-49FF-9D6B-DAA9184AE13A}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{F8DF4196-CCE5-4419-94F0-56D0F89FFD88}"/>
-    <hyperlink ref="H8" r:id="rId7" xr:uid="{9282ADB0-F1C9-4E82-A032-E03E4D33CC5F}"/>
-    <hyperlink ref="H9" r:id="rId8" xr:uid="{78E4936E-6154-4676-B777-BB41E41CA510}"/>
-    <hyperlink ref="H10" r:id="rId9" xr:uid="{EB89BBE2-6BBC-4043-8778-02058B78B6E1}"/>
-    <hyperlink ref="H11" r:id="rId10" xr:uid="{1CDB997A-7265-4C1F-896E-56EF5C692E03}"/>
-    <hyperlink ref="H2" r:id="rId11" xr:uid="{FEDE2EBB-F450-4FF8-A646-B65E67029069}"/>
+    <hyperlink ref="H4:H11" r:id="rId1" display="max.mustermann@example.com" xr:uid="{077A01C1-E489-4149-B981-81DAB0D867CD}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{C11D9D94-AD0C-46DA-A6DD-3C7F0E2C9559}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{6EE26CD2-963C-4EF1-8815-7C2C179EE829}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{FCB8C551-BF70-49FF-9D6B-DAA9184AE13A}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{F8DF4196-CCE5-4419-94F0-56D0F89FFD88}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{9282ADB0-F1C9-4E82-A032-E03E4D33CC5F}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{78E4936E-6154-4676-B777-BB41E41CA510}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{EB89BBE2-6BBC-4043-8778-02058B78B6E1}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{1CDB997A-7265-4C1F-896E-56EF5C692E03}"/>
+    <hyperlink ref="H3" r:id="rId10" xr:uid="{660703F7-726C-4AD9-923D-934962BF503C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fälschlicherweise doppeltes ToDoPanel gelöscht + Ausloggen bei Close-Schließen der App
</commit_message>
<xml_diff>
--- a/databases/DefaultUSERS.xlsx
+++ b/databases/DefaultUSERS.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="70">
   <si>
     <t>Max</t>
   </si>
@@ -717,7 +717,7 @@
         <v>1.0</v>
       </c>
       <c r="K2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>